<commit_message>
update api phase 1
</commit_message>
<xml_diff>
--- a/api.xlsx
+++ b/api.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OnTap\lapTrinhWebNangCao\doAn\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAB4A16F-592D-4259-83E6-B87CFA066E55}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B062528C-9F34-46C5-B85C-F98552B5C577}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{29F318D3-5C4C-4CE5-88B7-E78640BFBD62}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="39">
   <si>
     <t>token</t>
   </si>
@@ -148,6 +148,9 @@
   </si>
   <si>
     <t>(link video từ youtube only)</t>
+  </si>
+  <si>
+    <t>Bài viết hiện tại</t>
   </si>
 </sst>
 </file>
@@ -230,7 +233,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -240,26 +243,29 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -577,8 +583,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E152A520-3134-4ED3-AE63-41C78BA8D60A}">
   <dimension ref="A1:N61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="C56" sqref="C56:F56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -587,23 +593,23 @@
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
     </row>
     <row r="3" spans="1:14" ht="18" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
     </row>
     <row r="4" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -624,7 +630,7 @@
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="5" t="s">
         <v>17</v>
       </c>
       <c r="F5" s="4" t="s">
@@ -632,7 +638,7 @@
       </c>
     </row>
     <row r="6" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="8" t="s">
         <v>8</v>
       </c>
       <c r="B6" t="s">
@@ -646,7 +652,7 @@
       <c r="F6" s="9"/>
     </row>
     <row r="7" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="5"/>
+      <c r="A7" s="8"/>
       <c r="B7" t="s">
         <v>9</v>
       </c>
@@ -666,7 +672,7 @@
       <c r="N7" s="9"/>
     </row>
     <row r="8" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="5"/>
+      <c r="A8" s="8"/>
       <c r="B8" t="s">
         <v>14</v>
       </c>
@@ -675,7 +681,7 @@
       </c>
     </row>
     <row r="9" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="5"/>
+      <c r="A9" s="8"/>
       <c r="B9" t="s">
         <v>10</v>
       </c>
@@ -684,7 +690,7 @@
       </c>
     </row>
     <row r="10" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="5"/>
+      <c r="A10" s="8"/>
       <c r="B10" t="s">
         <v>16</v>
       </c>
@@ -700,25 +706,25 @@
       <c r="J10" s="9"/>
     </row>
     <row r="11" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="5"/>
+      <c r="A11" s="8"/>
       <c r="B11" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
     </row>
     <row r="13" spans="1:14" ht="18" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
     </row>
     <row r="14" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
@@ -739,7 +745,7 @@
       </c>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
-      <c r="E15" s="8" t="s">
+      <c r="E15" s="5" t="s">
         <v>17</v>
       </c>
       <c r="F15" s="4" t="s">
@@ -747,7 +753,7 @@
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="8" t="s">
         <v>8</v>
       </c>
       <c r="B16" t="s">
@@ -761,27 +767,27 @@
       <c r="F16" s="9"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A17" s="5"/>
+      <c r="A17" s="8"/>
       <c r="B17" t="s">
         <v>23</v>
       </c>
-      <c r="C17" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="9"/>
-      <c r="I17" s="9"/>
-      <c r="J17" s="9"/>
-      <c r="K17" s="9"/>
-      <c r="L17" s="9"/>
-      <c r="M17" s="9"/>
-      <c r="N17" s="9"/>
+      <c r="C17" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="14"/>
+      <c r="J17" s="14"/>
+      <c r="K17" s="14"/>
+      <c r="L17" s="14"/>
+      <c r="M17" s="14"/>
+      <c r="N17" s="14"/>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A18" s="5"/>
+      <c r="A18" s="8"/>
       <c r="B18" t="s">
         <v>10</v>
       </c>
@@ -790,7 +796,7 @@
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A19" s="5"/>
+      <c r="A19" s="8"/>
       <c r="B19" t="s">
         <v>16</v>
       </c>
@@ -806,28 +812,28 @@
       <c r="J19" s="9"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A20" s="5"/>
+      <c r="A20" s="8"/>
       <c r="B20" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="12" t="s">
+      <c r="C20" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A21" s="5"/>
+      <c r="A21" s="8"/>
     </row>
     <row r="23" spans="1:14" ht="18" x14ac:dyDescent="0.25">
-      <c r="A23" s="7" t="s">
+      <c r="A23" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B23" s="7"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
+      <c r="B23" s="11"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
     </row>
     <row r="24" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
@@ -848,11 +854,11 @@
       </c>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
-      <c r="E25" s="8"/>
+      <c r="E25" s="5"/>
       <c r="F25" s="4"/>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A26" s="5" t="s">
+      <c r="A26" s="8" t="s">
         <v>8</v>
       </c>
       <c r="B26" t="s">
@@ -866,27 +872,27 @@
       <c r="F26" s="9"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A27" s="5"/>
+      <c r="A27" s="8"/>
       <c r="B27" t="s">
         <v>25</v>
       </c>
-      <c r="C27" s="10" t="s">
+      <c r="C27" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="D27" s="10"/>
-      <c r="E27" s="10"/>
-      <c r="F27" s="10"/>
-      <c r="G27" s="10"/>
-      <c r="H27" s="10"/>
-      <c r="I27" s="10"/>
-      <c r="J27" s="10"/>
-      <c r="K27" s="10"/>
-      <c r="L27" s="10"/>
-      <c r="M27" s="10"/>
-      <c r="N27" s="10"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="6"/>
+      <c r="H27" s="6"/>
+      <c r="I27" s="6"/>
+      <c r="J27" s="6"/>
+      <c r="K27" s="6"/>
+      <c r="L27" s="6"/>
+      <c r="M27" s="6"/>
+      <c r="N27" s="6"/>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A28" s="5"/>
+      <c r="A28" s="8"/>
       <c r="B28" t="s">
         <v>27</v>
       </c>
@@ -895,39 +901,39 @@
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A29" s="5"/>
-      <c r="C29" s="10"/>
-      <c r="D29" s="10"/>
-      <c r="E29" s="10"/>
-      <c r="F29" s="10"/>
-      <c r="G29" s="10"/>
-      <c r="H29" s="10"/>
-      <c r="I29" s="10"/>
-      <c r="J29" s="10"/>
+      <c r="A29" s="8"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="6"/>
+      <c r="I29" s="6"/>
+      <c r="J29" s="6"/>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A30" s="5"/>
-      <c r="B30" s="13"/>
-      <c r="C30" s="13"/>
-      <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="13"/>
-      <c r="H30" s="13"/>
-      <c r="I30" s="13"/>
+      <c r="A30" s="8"/>
+      <c r="B30" s="12"/>
+      <c r="C30" s="12"/>
+      <c r="D30" s="12"/>
+      <c r="E30" s="12"/>
+      <c r="F30" s="12"/>
+      <c r="G30" s="12"/>
+      <c r="H30" s="12"/>
+      <c r="I30" s="12"/>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A31" s="5"/>
+      <c r="A31" s="8"/>
     </row>
     <row r="33" spans="1:10" ht="18" x14ac:dyDescent="0.25">
-      <c r="A33" s="7" t="s">
+      <c r="A33" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="B33" s="7"/>
-      <c r="C33" s="7"/>
-      <c r="D33" s="7"/>
-      <c r="E33" s="7"/>
-      <c r="F33" s="7"/>
+      <c r="B33" s="11"/>
+      <c r="C33" s="11"/>
+      <c r="D33" s="11"/>
+      <c r="E33" s="11"/>
+      <c r="F33" s="11"/>
     </row>
     <row r="34" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
@@ -948,11 +954,11 @@
       </c>
       <c r="C35" s="4"/>
       <c r="D35" s="4"/>
-      <c r="E35" s="8"/>
+      <c r="E35" s="5"/>
       <c r="F35" s="4"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A36" s="5" t="s">
+      <c r="A36" s="8" t="s">
         <v>8</v>
       </c>
       <c r="B36" t="s">
@@ -966,46 +972,46 @@
       <c r="F36" s="9"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A37" s="5"/>
-      <c r="C37" s="10"/>
-      <c r="D37" s="10"/>
-      <c r="E37" s="10"/>
-      <c r="F37" s="10"/>
-      <c r="G37" s="10"/>
-      <c r="H37" s="10"/>
-      <c r="I37" s="10"/>
-      <c r="J37" s="10"/>
+      <c r="A37" s="8"/>
+      <c r="C37" s="6"/>
+      <c r="D37" s="6"/>
+      <c r="E37" s="6"/>
+      <c r="F37" s="6"/>
+      <c r="G37" s="6"/>
+      <c r="H37" s="6"/>
+      <c r="I37" s="6"/>
+      <c r="J37" s="6"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A38" s="5"/>
-      <c r="B38" s="13"/>
-      <c r="C38" s="13"/>
-      <c r="D38" s="13"/>
-      <c r="E38" s="13"/>
-      <c r="F38" s="13"/>
-      <c r="G38" s="13"/>
-      <c r="H38" s="13"/>
-      <c r="I38" s="13"/>
+      <c r="A38" s="8"/>
+      <c r="B38" s="12"/>
+      <c r="C38" s="12"/>
+      <c r="D38" s="12"/>
+      <c r="E38" s="12"/>
+      <c r="F38" s="12"/>
+      <c r="G38" s="12"/>
+      <c r="H38" s="12"/>
+      <c r="I38" s="12"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A39" s="5"/>
+      <c r="A39" s="8"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A40" s="5"/>
-      <c r="C40" s="11"/>
+      <c r="A40" s="8"/>
+      <c r="C40" s="7"/>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A41" s="5"/>
+      <c r="A41" s="8"/>
     </row>
     <row r="43" spans="1:10" ht="18" x14ac:dyDescent="0.25">
-      <c r="A43" s="7" t="s">
+      <c r="A43" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="B43" s="7"/>
-      <c r="C43" s="7"/>
-      <c r="D43" s="7"/>
-      <c r="E43" s="7"/>
-      <c r="F43" s="7"/>
+      <c r="B43" s="11"/>
+      <c r="C43" s="11"/>
+      <c r="D43" s="11"/>
+      <c r="E43" s="11"/>
+      <c r="F43" s="11"/>
     </row>
     <row r="44" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
@@ -1026,11 +1032,11 @@
       </c>
       <c r="C45" s="4"/>
       <c r="D45" s="4"/>
-      <c r="E45" s="8"/>
+      <c r="E45" s="5"/>
       <c r="F45" s="4"/>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A46" s="5" t="s">
+      <c r="A46" s="8" t="s">
         <v>8</v>
       </c>
       <c r="B46" t="s">
@@ -1044,47 +1050,47 @@
       <c r="F46" s="9"/>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A47" s="5"/>
-      <c r="C47" s="10"/>
-      <c r="D47" s="10"/>
-      <c r="E47" s="10"/>
-      <c r="F47" s="10"/>
-      <c r="G47" s="10"/>
-      <c r="H47" s="10"/>
-      <c r="I47" s="10"/>
+      <c r="A47" s="8"/>
+      <c r="C47" s="6"/>
+      <c r="D47" s="6"/>
+      <c r="E47" s="6"/>
+      <c r="F47" s="6"/>
+      <c r="G47" s="6"/>
+      <c r="H47" s="6"/>
+      <c r="I47" s="6"/>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A48" s="5"/>
-      <c r="B48" s="12" t="s">
+      <c r="A48" s="8"/>
+      <c r="B48" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="C48" s="12"/>
-      <c r="D48" s="12"/>
-      <c r="E48" s="12"/>
-      <c r="F48" s="12"/>
-      <c r="G48" s="12"/>
-      <c r="H48" s="12"/>
-      <c r="I48" s="12"/>
+      <c r="C48" s="10"/>
+      <c r="D48" s="10"/>
+      <c r="E48" s="10"/>
+      <c r="F48" s="10"/>
+      <c r="G48" s="10"/>
+      <c r="H48" s="10"/>
+      <c r="I48" s="10"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A49" s="5"/>
+      <c r="A49" s="8"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A50" s="5"/>
-      <c r="C50" s="11"/>
+      <c r="A50" s="8"/>
+      <c r="C50" s="7"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A51" s="5"/>
+      <c r="A51" s="8"/>
     </row>
     <row r="53" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A53" s="7" t="s">
+      <c r="A53" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="B53" s="7"/>
-      <c r="C53" s="7"/>
-      <c r="D53" s="7"/>
-      <c r="E53" s="7"/>
-      <c r="F53" s="7"/>
+      <c r="B53" s="11"/>
+      <c r="C53" s="11"/>
+      <c r="D53" s="11"/>
+      <c r="E53" s="11"/>
+      <c r="F53" s="11"/>
     </row>
     <row r="54" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
@@ -1105,11 +1111,11 @@
       </c>
       <c r="C55" s="4"/>
       <c r="D55" s="4"/>
-      <c r="E55" s="8"/>
+      <c r="E55" s="5"/>
       <c r="F55" s="4"/>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A56" s="5" t="s">
+      <c r="A56" s="8" t="s">
         <v>8</v>
       </c>
       <c r="B56" t="s">
@@ -1123,40 +1129,53 @@
       <c r="F56" s="9"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A57" s="5"/>
-      <c r="C57" s="10"/>
-      <c r="D57" s="10"/>
-      <c r="E57" s="10"/>
-      <c r="F57" s="10"/>
-      <c r="G57" s="10"/>
-      <c r="H57" s="10"/>
-      <c r="I57" s="10"/>
+      <c r="A57" s="8"/>
+      <c r="C57" s="6"/>
+      <c r="D57" s="6"/>
+      <c r="E57" s="6"/>
+      <c r="F57" s="6"/>
+      <c r="G57" s="6"/>
+      <c r="H57" s="6"/>
+      <c r="I57" s="6"/>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A58" s="5"/>
-      <c r="B58" s="12" t="s">
+      <c r="A58" s="8"/>
+      <c r="B58" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="C58" s="12"/>
-      <c r="D58" s="12"/>
-      <c r="E58" s="12"/>
-      <c r="F58" s="12"/>
-      <c r="G58" s="12"/>
-      <c r="H58" s="12"/>
-      <c r="I58" s="12"/>
+      <c r="C58" s="10"/>
+      <c r="D58" s="10"/>
+      <c r="E58" s="10"/>
+      <c r="F58" s="10"/>
+      <c r="G58" s="10"/>
+      <c r="H58" s="10"/>
+      <c r="I58" s="10"/>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A59" s="5"/>
+      <c r="A59" s="8"/>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A60" s="5"/>
-      <c r="C60" s="11"/>
+      <c r="A60" s="8"/>
+      <c r="C60" s="7"/>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A61" s="5"/>
+      <c r="A61" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="C10:J10"/>
+    <mergeCell ref="C7:N7"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="A6:A11"/>
+    <mergeCell ref="A26:A31"/>
+    <mergeCell ref="C26:F26"/>
+    <mergeCell ref="A13:F13"/>
+    <mergeCell ref="A16:A21"/>
+    <mergeCell ref="C16:F16"/>
+    <mergeCell ref="C17:N17"/>
+    <mergeCell ref="C19:J19"/>
     <mergeCell ref="A56:A61"/>
     <mergeCell ref="C56:F56"/>
     <mergeCell ref="B58:I58"/>
@@ -1173,19 +1192,6 @@
     <mergeCell ref="B38:I38"/>
     <mergeCell ref="B30:I30"/>
     <mergeCell ref="A23:F23"/>
-    <mergeCell ref="A26:A31"/>
-    <mergeCell ref="C26:F26"/>
-    <mergeCell ref="A13:F13"/>
-    <mergeCell ref="A16:A21"/>
-    <mergeCell ref="C16:F16"/>
-    <mergeCell ref="C17:N17"/>
-    <mergeCell ref="C19:J19"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="A3:F3"/>
-    <mergeCell ref="C10:J10"/>
-    <mergeCell ref="C7:N7"/>
-    <mergeCell ref="C6:F6"/>
-    <mergeCell ref="A6:A11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>